<commit_message>
Simple Synchronous best vendor selector
</commit_message>
<xml_diff>
--- a/bin/catalog.xlsx
+++ b/bin/catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog Structure" sheetId="1" r:id="rId1"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1179,12 +1179,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
     <col min="4" max="4" width="16.75" customWidth="1"/>
     <col min="6" max="6" width="9.25" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Product Variant with duplicates check
</commit_message>
<xml_diff>
--- a/bin/catalog.xlsx
+++ b/bin/catalog.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog Structure" sheetId="1" r:id="rId1"/>
     <sheet name="Cow Milk" sheetId="2" r:id="rId2"/>
-    <sheet name="Flavoured Milk" sheetId="4" r:id="rId3"/>
-    <sheet name="Cone" sheetId="5" r:id="rId4"/>
+    <sheet name="Flavoured Milk" sheetId="3" r:id="rId3"/>
+    <sheet name="Cone" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>Root</t>
   </si>
@@ -76,154 +76,160 @@
     <t>MRP</t>
   </si>
   <si>
+    <t>Fat Percentage</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>MRPGOA</t>
+  </si>
+  <si>
+    <t>MRPPUNE</t>
+  </si>
+  <si>
+    <t>MRPMUMBAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arokya Milk  </t>
+  </si>
+  <si>
+    <t>Very healthy milk which helps in complete growth</t>
+  </si>
+  <si>
+    <t>Hatsun Coop</t>
+  </si>
+  <si>
+    <t>Arokya Milk 4.5% (500ml).jpg</t>
+  </si>
+  <si>
+    <t>500ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milk Cavin's </t>
+  </si>
+  <si>
+    <t>Delicious and healthy milk rich content of nutrients</t>
+  </si>
+  <si>
+    <t>Calvins Coop</t>
+  </si>
+  <si>
+    <t>Milk Cavin's 4.5%(500ml).jpg</t>
+  </si>
+  <si>
+    <t>Milk Hatsun</t>
+  </si>
+  <si>
+    <t>Tasty and Healthy milk</t>
+  </si>
+  <si>
+    <t>Milk Hatsun 3% (500ml).jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milk Mother Dairy </t>
+  </si>
+  <si>
+    <t>Nourishing and enriching milk</t>
+  </si>
+  <si>
+    <t>Mother Dairy</t>
+  </si>
+  <si>
+    <t>Milk Mother Dairy 3%(500ml).jpg</t>
+  </si>
+  <si>
+    <t>1000ml</t>
+  </si>
+  <si>
     <t>Fat %</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>MRPGOA</t>
-  </si>
-  <si>
-    <t>MRPPUNE</t>
-  </si>
-  <si>
-    <t>MRPMUMBAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arokya Milk  </t>
-  </si>
-  <si>
-    <t>Very healthy milk which helps in complete growth</t>
-  </si>
-  <si>
-    <t>Hatsun Coop</t>
-  </si>
-  <si>
-    <t>.\Catalog\CowMilk\Arokya Milk 4.5% (500ml).jpg</t>
-  </si>
-  <si>
-    <t>500ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milk Cavin's </t>
-  </si>
-  <si>
-    <t>Delicious and healthy milk rich content of nutrients</t>
-  </si>
-  <si>
-    <t>Calvins Coop</t>
-  </si>
-  <si>
-    <t>.\Catalog\CowMilk\Milk Cavin's 4.5%(500ml).jpg</t>
-  </si>
-  <si>
-    <t>Milk Hatsun</t>
-  </si>
-  <si>
-    <t>Tasty and Healthy milk</t>
-  </si>
-  <si>
-    <t>.\Catalog\CowMilk\Milk Hatsun 3% (500ml).jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milk Mother Dairy </t>
-  </si>
-  <si>
-    <t>Nourishing and enriching milk</t>
-  </si>
-  <si>
-    <t>Mother Dairy</t>
-  </si>
-  <si>
-    <t>.\Catalog\CowMilk\Milk Mother Dairy 3%(500ml).jpg</t>
+    <t>Energy</t>
   </si>
   <si>
     <t>MRPGoa</t>
   </si>
   <si>
+    <t>MRPPune</t>
+  </si>
+  <si>
     <t>MRPMumbai</t>
   </si>
   <si>
+    <t>Goa Dairy Flavoured Milk</t>
+  </si>
+  <si>
+    <t>Very Tasty</t>
+  </si>
+  <si>
+    <t>Goa Dairy</t>
+  </si>
+  <si>
+    <t>NestleNesquikChocolate(250ml).jpg</t>
+  </si>
+  <si>
+    <t>250ml</t>
+  </si>
+  <si>
+    <t>20kcal</t>
+  </si>
+  <si>
+    <t>Nestle Nesquik Chocolate</t>
+  </si>
+  <si>
+    <t>Sweet and Chocolaty</t>
+  </si>
+  <si>
+    <t>Nestle</t>
+  </si>
+  <si>
+    <t>GoaDairyFlavouredMilk(250ml).jpg</t>
+  </si>
+  <si>
+    <t>Nestle Nesquik Milk Additive</t>
+  </si>
+  <si>
+    <t>Chocolate Flavoured milk powder</t>
+  </si>
+  <si>
+    <t>NestleNesquikMilkAdditive(250gm).jpg</t>
+  </si>
+  <si>
+    <t>250gm</t>
+  </si>
+  <si>
+    <t>Nestle Nesquik Strawberry Milk Additive</t>
+  </si>
+  <si>
+    <t>Strawberry Flavoured milk powder</t>
+  </si>
+  <si>
+    <t>Nestle-nesquik-strawberry-flavor-flavored-milk-additive(250gm).jpg</t>
+  </si>
+  <si>
+    <t>Amul Butter Scotch</t>
+  </si>
+  <si>
+    <t>Butterscotch Cone</t>
+  </si>
+  <si>
     <t>Amul Coop</t>
   </si>
   <si>
-    <t>Goa Dairy</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>MRPPune</t>
-  </si>
-  <si>
-    <t>goaDairyFlavouredMilk</t>
-  </si>
-  <si>
-    <t>Very Tasty</t>
-  </si>
-  <si>
-    <t>.\Catalog\FlavouredMilk\nestleNesquikChocolate(250ml).jpg</t>
-  </si>
-  <si>
-    <t>250ml</t>
-  </si>
-  <si>
-    <t>20kcal</t>
-  </si>
-  <si>
-    <t>nestleNesquikChocolate</t>
-  </si>
-  <si>
-    <t>Sweet and Chocolaty</t>
-  </si>
-  <si>
-    <t>Nestle</t>
-  </si>
-  <si>
-    <t>.\Catalog\FlavouredMilk\goaDairyFlavouredMilk(250ml).jpg</t>
-  </si>
-  <si>
-    <t>nestleNesquikMilkAdditive</t>
-  </si>
-  <si>
-    <t>Chocolate Flavoured milk powder</t>
-  </si>
-  <si>
-    <t>.\Catalog\FlavouredMilk\nestleNesquikMilkAdditive(250gm).jpg</t>
-  </si>
-  <si>
-    <t>250gm</t>
-  </si>
-  <si>
-    <t>nestleNesquikStrawberry Milk Additive</t>
-  </si>
-  <si>
-    <t>Strawberry Flavoured milk powder</t>
-  </si>
-  <si>
-    <t>.\Catalog\FlavouredMilk\nestle-nesquik-strawberry-flavor-flavored-milk-additive(250gm).jpg</t>
-  </si>
-  <si>
-    <t>AmulButterScotch</t>
-  </si>
-  <si>
-    <t>Butterscotch Cone</t>
-  </si>
-  <si>
-    <t>.\Catalog\Cone\AmulButterScotch(30rs).jpg</t>
-  </si>
-  <si>
-    <t>FrostiesKingCone</t>
+    <t>AmulButterScotch(30rs).jpg</t>
+  </si>
+  <si>
+    <t>Frosties King Cone</t>
   </si>
   <si>
     <t>Frosties coop</t>
   </si>
   <si>
-    <t>.\Catalog\Cone\KapsFoodChocolate(30rs).jpg</t>
-  </si>
-  <si>
-    <t>KapsFoodChocolate</t>
+    <t>KapsFoodChocolate(30rs).jpg</t>
+  </si>
+  <si>
+    <t>Kaps Food Chocolate</t>
   </si>
   <si>
     <t>Chocolate Cone</t>
@@ -232,10 +238,10 @@
     <t>Kaps Food</t>
   </si>
   <si>
-    <t>.\Catalog\Cone\manzaHappyCones(25rs).jpg</t>
-  </si>
-  <si>
-    <t>manzaHappyCones</t>
+    <t>manzaHappyCones(25rs).jpg</t>
+  </si>
+  <si>
+    <t>manza Happy Cones</t>
   </si>
   <si>
     <t>Vannila Cone</t>
@@ -245,9 +251,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Fat Percentage</t>
   </si>
 </sst>
 </file>
@@ -618,33 +621,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -652,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -660,12 +661,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -673,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -681,7 +682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -689,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -706,18 +707,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -740,7 +741,7 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
@@ -755,9 +756,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -793,9 +794,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -831,9 +832,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -869,9 +870,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -907,9 +908,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -918,7 +919,7 @@
         <v>37</v>
       </c>
       <c r="D6">
-        <v>3949292933</v>
+        <v>5433235532</v>
       </c>
       <c r="E6" t="s">
         <v>38</v>
@@ -933,7 +934,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="J6">
         <v>21</v>
@@ -955,17 +956,12 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" max="2" width="32.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="77.75" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -988,27 +984,27 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
       </c>
       <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -1017,13 +1013,13 @@
         <v>47</v>
       </c>
       <c r="D2">
-        <v>343223456</v>
+        <v>989211122</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -1032,10 +1028,10 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K2">
         <v>15</v>
@@ -1047,24 +1043,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3">
-        <v>8322142459</v>
+        <v>223223456</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3">
         <v>22</v>
@@ -1073,10 +1069,10 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K3">
         <v>21</v>
@@ -1088,24 +1084,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" ht="15.75">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4">
-        <v>2325254446</v>
+        <v>224543323</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <v>30</v>
@@ -1114,10 +1110,10 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K4">
         <v>30</v>
@@ -1129,24 +1125,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5">
-        <v>3949292933</v>
+        <v>242425533</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5">
         <v>40</v>
@@ -1155,10 +1151,10 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K5">
         <v>40</v>
@@ -1179,18 +1175,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="9.25" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1213,39 +1204,39 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>343223456</v>
+        <v>123456732</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G2">
         <v>30</v>
@@ -1266,24 +1257,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3">
-        <v>8322142459</v>
+        <v>124321245</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>40</v>
@@ -1304,24 +1295,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4">
-        <v>2325254446</v>
+        <v>121452673</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G4">
         <v>40</v>
@@ -1342,24 +1333,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5">
+        <v>123453366</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
         <v>73</v>
-      </c>
-      <c r="D5">
-        <v>3949292933</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>71</v>
       </c>
       <c r="G5">
         <v>25</v>

</xml_diff>

<commit_message>
Company ID and Cats array from Excel Sheet
</commit_message>
<xml_diff>
--- a/bin/catalog.xlsx
+++ b/bin/catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog Structure" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Root</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>cid</t>
   </si>
 </sst>
 </file>
@@ -623,29 +626,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75">
+    <row r="3" spans="1:6">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75">
+    <row r="5" spans="1:6">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -653,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75">
+    <row r="6" spans="1:6">
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -661,12 +664,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
+    <row r="7" spans="1:6">
       <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -674,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
+    <row r="9" spans="1:6">
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -682,7 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75">
+    <row r="10" spans="1:6">
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -690,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75">
+    <row r="11" spans="1:6">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -705,20 +708,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -755,8 +758,11 @@
       <c r="L1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
+      <c r="M1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -793,8 +799,11 @@
       <c r="L2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+      <c r="M2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -831,8 +840,11 @@
       <c r="L3">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+      <c r="M3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -869,8 +881,11 @@
       <c r="L4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
+      <c r="M4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -907,8 +922,11 @@
       <c r="L5">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
+      <c r="M5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -944,6 +962,9 @@
       </c>
       <c r="L6">
         <v>22</v>
+      </c>
+      <c r="M6">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -953,15 +974,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1001,8 +1022,11 @@
       <c r="M1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75">
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1042,8 +1066,11 @@
       <c r="M2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75">
+      <c r="N2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1083,8 +1110,11 @@
       <c r="M3">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75">
+      <c r="N3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1124,8 +1154,11 @@
       <c r="M4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75">
+      <c r="N4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1164,6 +1197,9 @@
       </c>
       <c r="M5">
         <v>40</v>
+      </c>
+      <c r="N5">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1173,15 +1209,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="13" max="13" width="10.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1218,8 +1257,11 @@
       <c r="L1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
+      <c r="M1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1256,8 +1298,11 @@
       <c r="L2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+      <c r="M2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1294,8 +1339,11 @@
       <c r="L3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+      <c r="M3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1332,8 +1380,11 @@
       <c r="L4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
+      <c r="M4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1369,6 +1420,9 @@
       </c>
       <c r="L5">
         <v>25</v>
+      </c>
+      <c r="M5">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>